<commit_message>
FS-UC1, formel usecase template til UC mappe : check navningivningform
</commit_message>
<xml_diff>
--- a/Analysis/NavngivningForm.xlsx
+++ b/Analysis/NavngivningForm.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juyoung Choi\Desktop\1stYear Project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12624" windowHeight="6012"/>
   </bookViews>
   <sheets>
     <sheet name="navngivning" sheetId="1" r:id="rId1"/>
     <sheet name="revision historik" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A28:F43"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -533,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,7 +763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
UC1 reviewed with Sebastian + UC1-AD added
</commit_message>
<xml_diff>
--- a/Analysis/NavngivningForm.xlsx
+++ b/Analysis/NavngivningForm.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juyoung Choi\iCloudDrive\eclipse\flextur\Analysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10800" windowHeight="5856"/>
   </bookViews>
@@ -11,7 +16,6 @@
     <sheet name="revision historik" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A28:F43"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>Navngivning</t>
   </si>
@@ -195,6 +199,15 @@
   </si>
   <si>
     <t>Sekvens diagram</t>
+  </si>
+  <si>
+    <t>Aktivitetsdiagram</t>
+  </si>
+  <si>
+    <t>FS-UC#-navn-AD</t>
+  </si>
+  <si>
+    <t>FS-UC1-seHistorik-AD</t>
   </si>
 </sst>
 </file>
@@ -527,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E29"/>
+  <dimension ref="A2:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,172 +597,200 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
+    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+    <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>